<commit_message>
Update transcript questions to be open-ended
Remove specific topic assumptions (credit quality, acquisitions, etc.)
that may not exist in the data. Questions now ask for:
- Key themes
- Management discussion summaries
- Analyst focus areas
- Outlook and guidance (generally)
- Strategic priorities (without naming specific initiatives)

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/aegis_try_a_prompt_questions.xlsx
+++ b/aegis_try_a_prompt_questions.xlsx
@@ -545,7 +545,7 @@
       </c>
       <c r="B8" s="2" t="inlineStr">
         <is>
-          <t>What did RBC's CEO say about capital deployment priorities in Q3 2025?</t>
+          <t>What were the key themes from RBC's Q3 2025 earnings call?</t>
         </is>
       </c>
     </row>
@@ -557,7 +557,7 @@
       </c>
       <c r="B9" s="2" t="inlineStr">
         <is>
-          <t>How did TD management explain the increase in credit provisions in Q2 2025?</t>
+          <t>Summarize the management discussion from TD's Q2 2025 earnings call.</t>
         </is>
       </c>
     </row>
@@ -838,7 +838,7 @@
       </c>
       <c r="C17" s="2" t="inlineStr">
         <is>
-          <t>What outlook did RBC management provide on credit quality for 2025?</t>
+          <t>What outlook and guidance did RBC management provide in Q3 2025?</t>
         </is>
       </c>
     </row>
@@ -853,7 +853,7 @@
       </c>
       <c r="C18" s="2" t="inlineStr">
         <is>
-          <t>What did analysts ask about TD's Capital Markets performance in Q2 2025?</t>
+          <t>What were the main topics analysts asked about in TD's Q2 2025 earnings call?</t>
         </is>
       </c>
     </row>
@@ -868,7 +868,7 @@
       </c>
       <c r="C19" s="2" t="inlineStr">
         <is>
-          <t>How did BMO's CEO describe the Bank of the West integration progress in Q3 2025?</t>
+          <t>What strategic initiatives did BMO management highlight in Q3 2025?</t>
         </is>
       </c>
     </row>
@@ -883,7 +883,7 @@
       </c>
       <c r="C20" s="2" t="inlineStr">
         <is>
-          <t>Summarize what Scotiabank management said about International Banking in Q2 2025.</t>
+          <t>Summarize the key points from Scotiabank's Q2 2025 management discussion.</t>
         </is>
       </c>
     </row>
@@ -898,7 +898,7 @@
       </c>
       <c r="C21" s="2" t="inlineStr">
         <is>
-          <t>Compare how RBC and TD management discussed dividend policy in Q3 2025.</t>
+          <t>Compare the key themes from RBC and TD's Q3 2025 earnings calls.</t>
         </is>
       </c>
     </row>
@@ -1009,7 +1009,7 @@
       </c>
       <c r="B6" s="2" t="inlineStr">
         <is>
-          <t>What is RBC management's outlook on net interest margin for 2025?</t>
+          <t>What is the key guidance RBC management provided in Q3 2025?</t>
         </is>
       </c>
       <c r="C6" s="2" t="inlineStr">
@@ -1080,7 +1080,7 @@
       </c>
       <c r="B3" s="2" t="inlineStr">
         <is>
-          <t>Compare how RBC and TD management discussed credit quality in Q3 2025.</t>
+          <t>Compare the management outlook from RBC and TD in Q3 2025.</t>
         </is>
       </c>
       <c r="C3" s="2" t="inlineStr">
@@ -1181,7 +1181,7 @@
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>How did TD management explain the increase in credit provisions in Q2 2025?</t>
+          <t>How did TD management describe performance and outlook in Q2 2025?</t>
         </is>
       </c>
       <c r="C2" s="2" t="inlineStr">
@@ -1196,7 +1196,7 @@
       </c>
       <c r="B3" s="2" t="inlineStr">
         <is>
-          <t>How did RBC's CFO address analyst questions about expenses in Q3 2025?</t>
+          <t>How did RBC management respond to analyst concerns in Q3 2025?</t>
         </is>
       </c>
       <c r="C3" s="2" t="inlineStr">
@@ -1211,7 +1211,7 @@
       </c>
       <c r="B4" s="2" t="inlineStr">
         <is>
-          <t>How did BMO's CEO describe the rationale for recent acquisitions?</t>
+          <t>How did BMO management describe their strategic priorities in Q3 2025?</t>
         </is>
       </c>
       <c r="C4" s="2" t="inlineStr">
@@ -1312,7 +1312,7 @@
       </c>
       <c r="B3" s="2" t="inlineStr">
         <is>
-          <t>Summarize what Scotiabank management said about International Banking in Q3 2025.</t>
+          <t>Summarize the key themes from Scotiabank's Q3 2025 earnings call.</t>
         </is>
       </c>
       <c r="C3" s="2" t="inlineStr">
@@ -1357,7 +1357,7 @@
       </c>
       <c r="B6" s="2" t="inlineStr">
         <is>
-          <t>Summarize the key themes from RBC's Q3 2025 analyst Q&amp;A session.</t>
+          <t>Summarize the analyst Q&amp;A session from RBC's Q3 2025 earnings call.</t>
         </is>
       </c>
       <c r="C6" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Add landing page description to Excel file
New sheet 1 contains the Aegis landing page description text.
All other sheets shifted (now 7 total sheets).

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/aegis_try_a_prompt_questions.xlsx
+++ b/aegis_try_a_prompt_questions.xlsx
@@ -7,12 +7,13 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Landing Page" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Popup Questions" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Dropdown - What is" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Dropdown - Compare" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Dropdown - How did" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Dropdown - Summarize" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Landing Page Description" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Landing Page Questions" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Popup Questions" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Dropdown - What is" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Dropdown - Compare" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Dropdown - How did" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Dropdown - Summarize" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -68,13 +69,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -441,6 +443,42 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="100" customWidth="1" min="1" max="1"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Landing Page Description</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" ht="120" customHeight="1">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>Aegis serves finance professionals across RBC by providing a one-stop platform for financial insights and analysis on Canadian and US banks, enabling users to access comprehensive data through natural language conversations at their fingertips. It generates detailed responses drawing from Report to Shareholders (RTS), supplementary financial metrics, Pillar 3 capital disclosures, and earnings call transcripts covering 81 financial institutions globally, supporting both straightforward metric lookups and complex multi-bank comparisons. Users can focus on specific banks and time periods or ask broadly to get synthesized answers from multiple data sources, while pre-formatted reports help streamline monthly and quarterly deliverables for Investor Relations, Capital Markets, and Wealth Management teams.</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -454,12 +492,12 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" s="3" t="inlineStr">
         <is>
           <t>Database</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="3" t="inlineStr">
         <is>
           <t>Question</t>
         </is>
@@ -566,7 +604,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -586,17 +624,17 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" s="3" t="inlineStr">
         <is>
           <t>Database</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="3" t="inlineStr">
         <is>
           <t>#</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" s="3" t="inlineStr">
         <is>
           <t>Question</t>
         </is>
@@ -899,122 +937,6 @@
       <c r="C21" s="2" t="inlineStr">
         <is>
           <t>Compare the key themes from RBC and TD's Q3 2025 earnings calls.</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="5" customWidth="1" min="1" max="1"/>
-    <col width="80" customWidth="1" min="2" max="2"/>
-    <col width="15" customWidth="1" min="3" max="3"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>#</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Question</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Database</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="inlineStr">
-        <is>
-          <t>What is RBC's total Level 3 securities balance for Q2 2025?</t>
-        </is>
-      </c>
-      <c r="C2" s="2" t="inlineStr">
-        <is>
-          <t>RTS</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2" t="inlineStr">
-        <is>
-          <t>What is the CET1 ratio for RBC and National Bank in Q2 2025?</t>
-        </is>
-      </c>
-      <c r="C3" s="2" t="inlineStr">
-        <is>
-          <t>Pillar3</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2" t="inlineStr">
-        <is>
-          <t>What is the AUA and net income for RBC's Wealth Management segment in Q3 2025?</t>
-        </is>
-      </c>
-      <c r="C4" s="2" t="inlineStr">
-        <is>
-          <t>Supplementary</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" s="2" t="inlineStr">
-        <is>
-          <t>What is CIBC's diluted EPS, both reported and adjusted, for Q3 2025?</t>
-        </is>
-      </c>
-      <c r="C5" s="2" t="inlineStr">
-        <is>
-          <t>RTS</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="2" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" s="2" t="inlineStr">
-        <is>
-          <t>What is the key guidance RBC management provided in Q3 2025?</t>
-        </is>
-      </c>
-      <c r="C6" s="2" t="inlineStr">
-        <is>
-          <t>Transcripts</t>
         </is>
       </c>
     </row>
@@ -1043,17 +965,17 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" s="3" t="inlineStr">
         <is>
           <t>#</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="3" t="inlineStr">
         <is>
           <t>Question</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" s="3" t="inlineStr">
         <is>
           <t>Database</t>
         </is>
@@ -1065,12 +987,12 @@
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>Compare the efficiency ratio and ROE for TD and RBC in the latest quarter.</t>
+          <t>What is RBC's total Level 3 securities balance for Q2 2025?</t>
         </is>
       </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
-          <t>Supplementary</t>
+          <t>RTS</t>
         </is>
       </c>
     </row>
@@ -1080,12 +1002,12 @@
       </c>
       <c r="B3" s="2" t="inlineStr">
         <is>
-          <t>Compare the management outlook from RBC and TD in Q3 2025.</t>
+          <t>What is the CET1 ratio for RBC and National Bank in Q2 2025?</t>
         </is>
       </c>
       <c r="C3" s="2" t="inlineStr">
         <is>
-          <t>Transcripts</t>
+          <t>Pillar3</t>
         </is>
       </c>
     </row>
@@ -1095,12 +1017,12 @@
       </c>
       <c r="B4" s="2" t="inlineStr">
         <is>
-          <t>Compare the liquidity coverage ratio and leverage ratio across the Big Six banks for 2025.</t>
+          <t>What is the AUA and net income for RBC's Wealth Management segment in Q3 2025?</t>
         </is>
       </c>
       <c r="C4" s="2" t="inlineStr">
         <is>
-          <t>Pillar3</t>
+          <t>Supplementary</t>
         </is>
       </c>
     </row>
@@ -1110,12 +1032,12 @@
       </c>
       <c r="B5" s="2" t="inlineStr">
         <is>
-          <t>Compare investment fees and FICC revenue for RBC and BMO in Q3 2025.</t>
+          <t>What is CIBC's diluted EPS, both reported and adjusted, for Q3 2025?</t>
         </is>
       </c>
       <c r="C5" s="2" t="inlineStr">
         <is>
-          <t>Supplementary</t>
+          <t>RTS</t>
         </is>
       </c>
     </row>
@@ -1125,12 +1047,12 @@
       </c>
       <c r="B6" s="2" t="inlineStr">
         <is>
-          <t>Compare the key risk factors disclosed by TD and Scotiabank in Q2 2025.</t>
+          <t>What is the key guidance RBC management provided in Q3 2025?</t>
         </is>
       </c>
       <c r="C6" s="2" t="inlineStr">
         <is>
-          <t>RTS</t>
+          <t>Transcripts</t>
         </is>
       </c>
     </row>
@@ -1159,17 +1081,17 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" s="3" t="inlineStr">
         <is>
           <t>#</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="3" t="inlineStr">
         <is>
           <t>Question</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" s="3" t="inlineStr">
         <is>
           <t>Database</t>
         </is>
@@ -1181,12 +1103,12 @@
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>How did TD management describe performance and outlook in Q2 2025?</t>
+          <t>Compare the efficiency ratio and ROE for TD and RBC in the latest quarter.</t>
         </is>
       </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
-          <t>Transcripts</t>
+          <t>Supplementary</t>
         </is>
       </c>
     </row>
@@ -1196,7 +1118,7 @@
       </c>
       <c r="B3" s="2" t="inlineStr">
         <is>
-          <t>How did RBC management respond to analyst concerns in Q3 2025?</t>
+          <t>Compare the management outlook from RBC and TD in Q3 2025.</t>
         </is>
       </c>
       <c r="C3" s="2" t="inlineStr">
@@ -1211,12 +1133,12 @@
       </c>
       <c r="B4" s="2" t="inlineStr">
         <is>
-          <t>How did BMO management describe their strategic priorities in Q3 2025?</t>
+          <t>Compare the liquidity coverage ratio and leverage ratio across the Big Six banks for 2025.</t>
         </is>
       </c>
       <c r="C4" s="2" t="inlineStr">
         <is>
-          <t>Transcripts</t>
+          <t>Pillar3</t>
         </is>
       </c>
     </row>
@@ -1226,12 +1148,12 @@
       </c>
       <c r="B5" s="2" t="inlineStr">
         <is>
-          <t>How did TD's risk-weighted assets change from Q1 to Q2 2025?</t>
+          <t>Compare investment fees and FICC revenue for RBC and BMO in Q3 2025.</t>
         </is>
       </c>
       <c r="C5" s="2" t="inlineStr">
         <is>
-          <t>Pillar3</t>
+          <t>Supplementary</t>
         </is>
       </c>
     </row>
@@ -1241,7 +1163,7 @@
       </c>
       <c r="B6" s="2" t="inlineStr">
         <is>
-          <t>How did CIBC describe their risk management strategy in Q2 2025?</t>
+          <t>Compare the key risk factors disclosed by TD and Scotiabank in Q2 2025.</t>
         </is>
       </c>
       <c r="C6" s="2" t="inlineStr">
@@ -1275,17 +1197,133 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" s="3" t="inlineStr">
         <is>
           <t>#</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="3" t="inlineStr">
         <is>
           <t>Question</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" s="3" t="inlineStr">
+        <is>
+          <t>Database</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="inlineStr">
+        <is>
+          <t>How did TD management describe performance and outlook in Q2 2025?</t>
+        </is>
+      </c>
+      <c r="C2" s="2" t="inlineStr">
+        <is>
+          <t>Transcripts</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="inlineStr">
+        <is>
+          <t>How did RBC management respond to analyst concerns in Q3 2025?</t>
+        </is>
+      </c>
+      <c r="C3" s="2" t="inlineStr">
+        <is>
+          <t>Transcripts</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="inlineStr">
+        <is>
+          <t>How did BMO management describe their strategic priorities in Q3 2025?</t>
+        </is>
+      </c>
+      <c r="C4" s="2" t="inlineStr">
+        <is>
+          <t>Transcripts</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="inlineStr">
+        <is>
+          <t>How did TD's risk-weighted assets change from Q1 to Q2 2025?</t>
+        </is>
+      </c>
+      <c r="C5" s="2" t="inlineStr">
+        <is>
+          <t>Pillar3</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="inlineStr">
+        <is>
+          <t>How did CIBC describe their risk management strategy in Q2 2025?</t>
+        </is>
+      </c>
+      <c r="C6" s="2" t="inlineStr">
+        <is>
+          <t>RTS</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="5" customWidth="1" min="1" max="1"/>
+    <col width="80" customWidth="1" min="2" max="2"/>
+    <col width="15" customWidth="1" min="3" max="3"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="3" t="inlineStr">
+        <is>
+          <t>#</t>
+        </is>
+      </c>
+      <c r="B1" s="3" t="inlineStr">
+        <is>
+          <t>Question</t>
+        </is>
+      </c>
+      <c r="C1" s="3" t="inlineStr">
         <is>
           <t>Database</t>
         </is>

</xml_diff>